<commit_message>
updated with PUT-final day
</commit_message>
<xml_diff>
--- a/RestAssuredTest/src/test/resources/data/testDataTwinkle.xlsx
+++ b/RestAssuredTest/src/test/resources/data/testDataTwinkle.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bsethur\Desktop\restassured\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42545AF5-3530-4765-9DD0-AA254A0FB1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC044338-5213-480C-84EB-5C4429AE81BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11385" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Export Summary" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="193">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -617,13 +617,16 @@
     <t>grade</t>
   </si>
   <si>
-    <t>07-26-2023 06:29:27</t>
-  </si>
-  <si>
     <t>Put_GradeSubmission_InValid</t>
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>07-29-2023 05:29:27</t>
+  </si>
+  <si>
+    <t>07-27-2023 06:29:27</t>
   </si>
 </sst>
 </file>
@@ -690,11 +693,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="20"/>
-      <name val="Menlo Regular"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color indexed="21"/>
       <name val="Menlo Regular"/>
     </font>
@@ -709,6 +707,12 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2A00FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1035,27 +1039,27 @@
     <xf numFmtId="49" fontId="9" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="13" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2485,7 +2489,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
@@ -2528,7 +2532,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
@@ -2576,8 +2580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB15F78-E8CE-4EC6-AD53-95101F1FBF41}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2619,8 +2623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{331DE8BD-0DF4-44E6-8CB0-BB9E0507995C}">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2630,8 +2634,11 @@
     <col min="3" max="3" width="31.5703125" customWidth="1"/>
     <col min="4" max="4" width="30.85546875" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" customWidth="1"/>
-    <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="30">
@@ -2662,13 +2669,13 @@
       <c r="I1" s="19" t="s">
         <v>130</v>
       </c>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="42" t="s">
         <v>186</v>
       </c>
-      <c r="K1" s="43" t="s">
+      <c r="K1" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="L1" s="44" t="s">
+      <c r="L1" s="43" t="s">
         <v>188</v>
       </c>
       <c r="M1" s="19" t="s">
@@ -2679,7 +2686,7 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="16.5">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="41" t="s">
         <v>184</v>
       </c>
       <c r="B2" s="21" t="s">
@@ -2712,7 +2719,7 @@
       <c r="N2" s="29"/>
     </row>
     <row r="3" spans="1:14" ht="16.5">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="41" t="s">
         <v>180</v>
       </c>
       <c r="B3" s="21" t="s">
@@ -2745,7 +2752,7 @@
       <c r="N3" s="30"/>
     </row>
     <row r="4" spans="1:14" ht="16.5">
-      <c r="A4" s="42" t="s">
+      <c r="A4" s="41" t="s">
         <v>185</v>
       </c>
       <c r="B4" s="21" t="s">
@@ -2776,10 +2783,10 @@
         <v>177</v>
       </c>
       <c r="K4" s="33" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M4" s="21" t="s">
         <v>138</v>
@@ -2789,8 +2796,8 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="16.5">
-      <c r="A5" s="42" t="s">
-        <v>190</v>
+      <c r="A5" s="44" t="s">
+        <v>189</v>
       </c>
       <c r="B5" s="21" t="s">
         <v>183</v>
@@ -2829,7 +2836,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="16.5">
-      <c r="A6" s="42"/>
+      <c r="A6" s="41"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
       <c r="D6" s="33"/>
@@ -2842,7 +2849,7 @@
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="1:14" ht="16.5">
-      <c r="A7" s="42"/>
+      <c r="A7" s="41"/>
       <c r="B7" s="21"/>
       <c r="C7" s="21"/>
       <c r="D7" s="33"/>
@@ -2856,7 +2863,7 @@
     </row>
     <row r="20" spans="5:5">
       <c r="E20" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
   </sheetData>
@@ -4444,8 +4451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -4506,7 +4513,7 @@
         <v>133</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>134</v>
+        <v>191</v>
       </c>
       <c r="E2" s="21" t="s">
         <v>83</v>
@@ -4537,7 +4544,7 @@
         <v>133</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>134</v>
+        <v>191</v>
       </c>
       <c r="E3" s="21" t="s">
         <v>83</v>
@@ -4570,7 +4577,7 @@
         <v>133</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>134</v>
+        <v>191</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>83</v>
@@ -4640,7 +4647,7 @@
         <v>133</v>
       </c>
       <c r="D6" s="33" t="s">
-        <v>134</v>
+        <v>191</v>
       </c>
       <c r="E6" s="21" t="s">
         <v>83</v>
@@ -4698,7 +4705,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="21" t="s">
         <v>146</v>
       </c>
       <c r="B8" s="21"/>
@@ -4717,7 +4724,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" ht="15" customHeight="1">
-      <c r="A9" s="37" t="s">
+      <c r="A9" s="21" t="s">
         <v>148</v>
       </c>
       <c r="B9" s="21"/>
@@ -4794,11 +4801,11 @@
       <c r="A1" s="21" t="s">
         <v>150</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
       <c r="G1" s="21" t="s">
         <v>25</v>
       </c>
@@ -4807,11 +4814,11 @@
       <c r="A2" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="21" t="s">
         <v>25</v>
       </c>
@@ -4820,11 +4827,11 @@
       <c r="A3" s="21" t="s">
         <v>152</v>
       </c>
-      <c r="B3" s="38"/>
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
       <c r="G3" s="21" t="s">
         <v>153</v>
       </c>
@@ -4833,11 +4840,11 @@
       <c r="A4" s="21" t="s">
         <v>154</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
       <c r="G4" s="21" t="s">
         <v>153</v>
       </c>
@@ -4846,11 +4853,11 @@
       <c r="A5" s="21" t="s">
         <v>155</v>
       </c>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
+      <c r="B5" s="37"/>
+      <c r="C5" s="37"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="37"/>
+      <c r="F5" s="37"/>
       <c r="G5" s="21" t="s">
         <v>156</v>
       </c>
@@ -4859,11 +4866,11 @@
       <c r="A6" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="B6" s="38"/>
-      <c r="C6" s="38"/>
-      <c r="D6" s="38"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="38"/>
+      <c r="B6" s="37"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
       <c r="G6" s="21" t="s">
         <v>156</v>
       </c>
@@ -4872,11 +4879,11 @@
       <c r="A7" s="21" t="s">
         <v>158</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
+      <c r="B7" s="37"/>
+      <c r="C7" s="37"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="37"/>
+      <c r="F7" s="37"/>
       <c r="G7" s="21" t="s">
         <v>7</v>
       </c>
@@ -4885,11 +4892,11 @@
       <c r="A8" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="B8" s="38"/>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="37"/>
+      <c r="F8" s="37"/>
       <c r="G8" s="21" t="s">
         <v>7</v>
       </c>
@@ -4910,7 +4917,7 @@
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
       <c r="F10" s="19"/>
-      <c r="G10" s="38"/>
+      <c r="G10" s="37"/>
     </row>
     <row r="11" spans="1:7" ht="15" customHeight="1">
       <c r="A11" s="21" t="s">
@@ -4919,7 +4926,7 @@
       <c r="B11" s="22" t="s">
         <v>161</v>
       </c>
-      <c r="C11" s="39">
+      <c r="C11" s="38">
         <v>11295</v>
       </c>
       <c r="D11" s="23" t="s">
@@ -4972,7 +4979,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="39" t="s">
         <v>12</v>
       </c>
       <c r="B1" t="s">
@@ -4988,7 +4995,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="40" t="s">
         <v>165</v>
       </c>
       <c r="B3">

</xml_diff>